<commit_message>
Refractoring to fit my personal dataset
</commit_message>
<xml_diff>
--- a/prostate_cancer_nomograms/data/mock_dataset.xlsx
+++ b/prostate_cancer_nomograms/data/mock_dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxen\Desktop\Genie Physique\Github\ProstateCancerNomograms\prostate_cancer_nomograms\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4615028-C71C-44C8-A756-F14D457C3907}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEE808C1-61A2-4A0D-A313-461899BDFA88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,21 +27,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
   <si>
-    <t>Age</t>
-  </si>
-  <si>
     <t>Patient</t>
   </si>
   <si>
-    <t>PSA</t>
-  </si>
-  <si>
-    <t>Primary Gleason</t>
-  </si>
-  <si>
-    <t>Secondary Gleason</t>
-  </si>
-  <si>
     <t>Surgical Margin Status</t>
   </si>
   <si>
@@ -57,15 +45,6 @@
     <t>Free Months</t>
   </si>
   <si>
-    <t>Clinical Tumor Stage</t>
-  </si>
-  <si>
-    <t>Number of Positive Cores</t>
-  </si>
-  <si>
-    <t>Number of Negative Cores</t>
-  </si>
-  <si>
     <t>T2a</t>
   </si>
   <si>
@@ -79,6 +58,27 @@
   </si>
   <si>
     <t>True</t>
+  </si>
+  <si>
+    <t>âge au dx</t>
+  </si>
+  <si>
+    <t>Diag_PSA</t>
+  </si>
+  <si>
+    <t>Gleason primaire Bx</t>
+  </si>
+  <si>
+    <t>Gleason secondaire Bx</t>
+  </si>
+  <si>
+    <t>Stade clinique</t>
+  </si>
+  <si>
+    <t>NbCtePositive</t>
+  </si>
+  <si>
+    <t>NbCteNegative</t>
   </si>
 </sst>
 </file>
@@ -399,7 +399,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -421,43 +421,43 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="J1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="K1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="L1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" t="s">
-        <v>8</v>
-      </c>
       <c r="M1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -477,7 +477,7 @@
         <v>5</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="G2">
         <v>2</v>
@@ -486,16 +486,16 @@
         <v>2</v>
       </c>
       <c r="I2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="J2" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="K2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="L2" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="M2">
         <v>8</v>
@@ -518,7 +518,7 @@
         <v>4</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="G3">
         <v>5</v>
@@ -527,16 +527,16 @@
         <v>5</v>
       </c>
       <c r="I3" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="J3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="K3" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="L3" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="M3">
         <v>20</v>
@@ -559,7 +559,7 @@
         <v>5</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G4">
         <v>10</v>
@@ -568,16 +568,16 @@
         <v>5</v>
       </c>
       <c r="I4" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="J4" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="K4" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="L4" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="M4">
         <v>40</v>

</xml_diff>